<commit_message>
Added getTruckDistances2 WB doc
added xlsx version of BB + WB tests of getTruckDistances2 and finalised getTruckByReference test xlsx
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_GetTruckByReference.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_GetTruckByReference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cescadelacruz/Documents/GitHub/SUM23-SFT221-NAA-4/Documents/Testing/TestsDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE123F48-BD55-4A43-A521-C82133C9FB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F274763C-EDB2-A842-9979-7305EA43260C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>SFT 221</t>
   </si>
@@ -89,14 +89,7 @@
     <t>Anna Francesca Dela Cruz (Cesca)</t>
   </si>
   <si>
-    <t>TestGetTruckByReference</t>
-  </si>
-  <si>
     <t>Blackbox and Whitebox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This function retrieves a pointer to a Truck based on its routeSymbol. The function accesses the routeSymbol inside the nested structs of current and iterates over them. If the routeSymbol of a Truck matches the argument of the routeSymbol parameter (either 2, 4, or 8), then the pointer to the matching Truck is returned. If no matching truck is found, it returns a NULL pointer.
-This function is used to sort the trucks based on their volume and weight, and their distance from the destination. </t>
   </si>
   <si>
     <t>BB_TestGetTruckByReference1</t>
@@ -160,10 +153,6 @@
   </si>
   <si>
     <t>Return NULL when the pointer to Fleet is NULL</t>
-  </si>
-  <si>
-    <t>struct Fleet *nullFleet = NULL;
-getTruckByReference(nullFleet, 2);</t>
   </si>
   <si>
     <t>Output = NULL
@@ -257,6 +246,24 @@
     <t>Check function does not return first truck second truck if all routeSymbols are the same</t>
   </si>
   <si>
+    <t>This function retrieves a pointer to a Truck based on its routeSymbol. The function accesses the routeSymbol inside the nested structs of current and iterates over them. If the routeSymbol of a Truck matches the argument of the routeSymbol parameter (either 2, 4, or 8), then the pointer to the matching Truck is returned. If no matching truck is found, it returns a NULL pointer.
+This function is used to sort the trucks based on their volume and weight, and their distance from the destination. 
+The purpose of the test is to ensure the function returns the correct Truck pointer based on the argument of the routeSymbol parameter.</t>
+  </si>
+  <si>
+    <t>getTrucksByReferencetests</t>
+  </si>
+  <si>
+    <t>struct Fleet *nullFleet;
+			nullFleet.G.route.routeSymbol = NULL;
+			nullFleet.B.route.routeSymbol = NULL;
+			nullFleet.Y.route.routeSymbol = NULL;
+getTruckByReference(&amp;nullFleet, 2);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass </t>
+  </si>
+  <si>
     <t>Blackbox Setup:
 1.	Copy the Fleet struct (parameter 1) that nests the 3 Truck structs. 
 2.	Ensure that each Truck struct has a unique routeSymbol assigned (e.g. 4, 2, and 8). 
@@ -264,7 +271,7 @@
 4.	Call getTruckByReference with the copied Fleet struct and the routeSymbol arguments.
 5.	Declare and define a pointer that is assigned the Truck struct we expect to be returned.
 6.	Create assertions to compare the return value with the expected value and validate the returned Truck pointer.
-Whitebox Setup
+Whitebox Setup:
 1.Copy the Fleet struct (parameter 1) that nests the 3 Truck structs. 
 2.	Ensure that each Truck struct has a unique routeSymbol assigned (e.g. 4, 2, and 8). 
 3.	Define the argument for the routeSymbol parameter (parameter 2). 
@@ -460,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -484,6 +491,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -815,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -825,120 +835,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="19">
         <v>4</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
+      <c r="B7" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21"/>
-    </row>
-    <row r="9" spans="1:9" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" ht="174" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
-    </row>
-    <row r="10" spans="1:9" ht="254" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" ht="278" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -961,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -977,14 +987,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
+      <c r="A1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1003,152 +1013,168 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="8"/>
+        <v>45</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="8"/>
+        <v>48</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="8"/>
+        <v>45</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="8"/>
+        <v>45</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F11" s="3"/>
@@ -1266,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBEBE5-E65B-48FE-ACB2-E1CF3882866A}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1283,14 +1309,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
+      <c r="A1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1309,44 +1335,48 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="F3" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
@@ -1409,52 +1439,55 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="M28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.2">
@@ -1502,12 +1535,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1516,7 +1543,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008641478389A1824A98F5C5E0B6162E5F" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9ef4b42a3ed9448361827c423e89ef89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81b064ac-ebcb-49a1-93f6-e61f75bebfa7" xmlns:ns3="717d1b07-b5a1-4bb5-9d40-3a9b6c764643" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0bb8b9f62ca6562dff4b6b6c0721aa08" ns2:_="" ns3:_="">
     <xsd:import namespace="81b064ac-ebcb-49a1-93f6-e61f75bebfa7"/>
@@ -1687,24 +1714,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1712,7 +1728,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A5AAF0-BBBC-48E3-AADB-8E4922D37D7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1729,4 +1745,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
made test names on getTruckByRef consistent
...consistent with test names on matrix
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_GetTruckByReference.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_GetTruckByReference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cescadelacruz/Documents/GitHub/SUM23-SFT221-NAA-4/Documents/Testing/TestsDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F274763C-EDB2-A842-9979-7305EA43260C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686B3F2A-67F6-974E-8ED5-7F2059E2B99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -92,30 +92,6 @@
     <t>Blackbox and Whitebox</t>
   </si>
   <si>
-    <t>BB_TestGetTruckByReference1</t>
-  </si>
-  <si>
-    <t>BB_TestGetTruckByReference2</t>
-  </si>
-  <si>
-    <t>BB_TestGetTruckByReference3</t>
-  </si>
-  <si>
-    <t>BB_TestGetTruckByReference4</t>
-  </si>
-  <si>
-    <t>BB_TestGetTruckByReference5</t>
-  </si>
-  <si>
-    <t>BB_TestGetTruckByReference6</t>
-  </si>
-  <si>
-    <t>BB_TestGetTruckByReference7</t>
-  </si>
-  <si>
-    <t>BB_TestGetTruckByReference8</t>
-  </si>
-  <si>
     <t>Pass/Fail</t>
   </si>
   <si>
@@ -126,15 +102,6 @@
   </si>
   <si>
     <t>Check function returns pointer to third truck</t>
-  </si>
-  <si>
-    <t>FUNCTION: GetTruckByReference</t>
-  </si>
-  <si>
-    <t>WB_TestGetTruckByReference1</t>
-  </si>
-  <si>
-    <t>WB_TestGetTruckByReference2</t>
   </si>
   <si>
     <t>Find pointer to truck with only 1 truck in the Fleet struct.</t>
@@ -279,6 +246,39 @@
 Declare and define a pointer that is assigned the Truck struct we expect to be returned.
 6.	Create assertion to compare the return value with the expected value and validate the returned Truck pointer.
 7. Create assertion to check if NULL was returned.</t>
+  </si>
+  <si>
+    <t>WB_getTruckByReference1</t>
+  </si>
+  <si>
+    <t>WB_getTruckByReference2</t>
+  </si>
+  <si>
+    <t>FUNCTION: getTruckByReference</t>
+  </si>
+  <si>
+    <t>BB_getTruckByReference1</t>
+  </si>
+  <si>
+    <t>BB_getTruckByReference2</t>
+  </si>
+  <si>
+    <t>BB_getTruckByReference3</t>
+  </si>
+  <si>
+    <t>BB_getTruckByReference4</t>
+  </si>
+  <si>
+    <t>BB_getTruckByReference5</t>
+  </si>
+  <si>
+    <t>BB_getTruckByReference6</t>
+  </si>
+  <si>
+    <t>BB_getTruckByReference7</t>
+  </si>
+  <si>
+    <t>BB_getTruckByReference8</t>
   </si>
 </sst>
 </file>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -895,7 +895,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -925,7 +925,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -940,7 +940,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -988,7 +988,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -1013,167 +1013,167 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="E4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1294,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBEBE5-E65B-48FE-ACB2-E1CF3882866A}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1310,7 +1310,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -1335,47 +1335,47 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1475,7 +1475,7 @@
     <row r="28" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E28" s="3"/>
       <c r="M28" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
made "pass" fields green
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_GetTruckByReference.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_GetTruckByReference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cescadelacruz/Documents/GitHub/SUM23-SFT221-NAA-4/Documents/Testing/TestsDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686B3F2A-67F6-974E-8ED5-7F2059E2B99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2342907E-17D0-1C47-866D-FF12EABE217D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +333,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -492,9 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -542,6 +545,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:I7"/>
     </sheetView>
   </sheetViews>
@@ -835,120 +841,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>4</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="22"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:9" ht="174" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="22"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:9" ht="278" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -971,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -987,14 +993,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1032,7 +1038,7 @@
       <c r="E3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1052,7 +1058,7 @@
       <c r="E4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1072,7 +1078,7 @@
       <c r="E5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1092,7 +1098,7 @@
       <c r="E6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1112,7 +1118,7 @@
       <c r="E7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1132,7 +1138,7 @@
       <c r="E8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1152,7 +1158,7 @@
       <c r="E9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1172,7 +1178,7 @@
       <c r="E10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1294,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBEBE5-E65B-48FE-ACB2-E1CF3882866A}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1309,14 +1315,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1354,7 +1360,7 @@
       <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1374,7 +1380,7 @@
       <c r="E4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="26" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1535,12 +1541,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1715,15 +1718,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1748,18 +1763,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>